<commit_message>
add a rule to c5
bok
</commit_message>
<xml_diff>
--- a/save/c5/c5 seats.xlsx
+++ b/save/c5/c5 seats.xlsx
@@ -879,7 +879,7 @@
       <c r="J1" s="24" t="n"/>
       <c r="K1" s="25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 06 Sep, 2022</t>
+          <t xml:space="preserve"> 18 Sep, 2022</t>
         </is>
       </c>
       <c r="L1" s="24" t="n"/>
@@ -930,7 +930,7 @@
       </c>
       <c r="B4" s="13" t="inlineStr">
         <is>
-          <t>迟涵予</t>
+          <t>白宇轩</t>
         </is>
       </c>
       <c r="C4" s="21" t="inlineStr">
@@ -945,37 +945,37 @@
       </c>
       <c r="E4" s="14" t="inlineStr">
         <is>
+          <t>范青桐</t>
+        </is>
+      </c>
+      <c r="F4" s="21" t="inlineStr">
+        <is>
+          <t>邱晨朔</t>
+        </is>
+      </c>
+      <c r="G4" s="36" t="inlineStr">
+        <is>
+          <t>过道</t>
+        </is>
+      </c>
+      <c r="H4" s="14" t="inlineStr">
+        <is>
+          <t>廖从云</t>
+        </is>
+      </c>
+      <c r="I4" s="15" t="inlineStr">
+        <is>
+          <t>边麓元</t>
+        </is>
+      </c>
+      <c r="J4" s="36" t="inlineStr">
+        <is>
+          <t>过道</t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="inlineStr">
+        <is>
           <t>龚搏扬</t>
-        </is>
-      </c>
-      <c r="F4" s="21" t="inlineStr">
-        <is>
-          <t>石清泓</t>
-        </is>
-      </c>
-      <c r="G4" s="36" t="inlineStr">
-        <is>
-          <t>过道</t>
-        </is>
-      </c>
-      <c r="H4" s="14" t="inlineStr">
-        <is>
-          <t>李星宸</t>
-        </is>
-      </c>
-      <c r="I4" s="15" t="inlineStr">
-        <is>
-          <t>林彦含</t>
-        </is>
-      </c>
-      <c r="J4" s="36" t="inlineStr">
-        <is>
-          <t>过道</t>
-        </is>
-      </c>
-      <c r="K4" s="1" t="inlineStr">
-        <is>
-          <t>吴周毅</t>
         </is>
       </c>
       <c r="L4" s="32" t="n"/>
@@ -985,40 +985,40 @@
       <c r="A5" s="28" t="n"/>
       <c r="B5" s="13" t="inlineStr">
         <is>
-          <t>程启航</t>
+          <t>卢逸</t>
         </is>
       </c>
       <c r="C5" s="14" t="inlineStr">
         <is>
-          <t>丁鹏元</t>
+          <t>陈元畅</t>
         </is>
       </c>
       <c r="D5" s="37" t="n"/>
       <c r="E5" s="14" t="inlineStr">
         <is>
-          <t>廖从云</t>
+          <t>张宸瑞</t>
         </is>
       </c>
       <c r="F5" s="19" t="inlineStr">
         <is>
-          <t>边麓元</t>
+          <t>曾韦翔</t>
         </is>
       </c>
       <c r="G5" s="37" t="n"/>
       <c r="H5" s="14" t="inlineStr">
         <is>
-          <t>王昊天</t>
+          <t>詹悦</t>
         </is>
       </c>
       <c r="I5" s="1" t="inlineStr">
         <is>
-          <t>张宸瑞</t>
+          <t>林彦含</t>
         </is>
       </c>
       <c r="J5" s="37" t="n"/>
       <c r="K5" s="14" t="inlineStr">
         <is>
-          <t>郑俊永</t>
+          <t>龙飞宇</t>
         </is>
       </c>
       <c r="L5" s="14" t="n"/>
@@ -1032,45 +1032,45 @@
       <c r="A6" s="28" t="n"/>
       <c r="B6" s="16" t="inlineStr">
         <is>
-          <t>龙飞宇</t>
+          <t>骆子墨</t>
         </is>
       </c>
       <c r="C6" s="14" t="inlineStr">
         <is>
-          <t>曾韦翔</t>
+          <t>赖思轩</t>
         </is>
       </c>
       <c r="D6" s="37" t="n"/>
       <c r="E6" s="19" t="inlineStr">
         <is>
-          <t>范青桐</t>
+          <t>程启航</t>
         </is>
       </c>
       <c r="F6" s="19" t="inlineStr">
         <is>
-          <t>邱晨朔</t>
+          <t>李星宸</t>
         </is>
       </c>
       <c r="G6" s="37" t="n"/>
       <c r="H6" s="19" t="inlineStr">
         <is>
-          <t>骆子墨</t>
+          <t>黄婧涵</t>
         </is>
       </c>
       <c r="I6" s="19" t="inlineStr">
         <is>
-          <t>赖思轩</t>
+          <t>石清泓</t>
         </is>
       </c>
       <c r="J6" s="37" t="n"/>
       <c r="K6" s="19" t="inlineStr">
         <is>
-          <t>陈元畅</t>
+          <t>迟涵予</t>
         </is>
       </c>
       <c r="L6" s="19" t="inlineStr">
         <is>
-          <t>张扬</t>
+          <t>郑俊永</t>
         </is>
       </c>
       <c r="M6" s="33" t="n"/>
@@ -1079,45 +1079,45 @@
       <c r="A7" s="29" t="n"/>
       <c r="B7" s="17" t="inlineStr">
         <is>
-          <t>杨熙宇</t>
+          <t>杜心扬</t>
         </is>
       </c>
       <c r="C7" s="18" t="inlineStr">
         <is>
-          <t>陈李石农</t>
+          <t>章淏博</t>
         </is>
       </c>
       <c r="D7" s="38" t="n"/>
       <c r="E7" s="17" t="inlineStr">
         <is>
-          <t>杜心扬</t>
+          <t>吴周毅</t>
         </is>
       </c>
       <c r="F7" s="36" t="inlineStr">
         <is>
-          <t>章淏博</t>
+          <t>杨熙宇</t>
         </is>
       </c>
       <c r="G7" s="38" t="n"/>
       <c r="H7" s="18" t="inlineStr">
         <is>
-          <t>白宇轩</t>
+          <t>张扬</t>
         </is>
       </c>
       <c r="I7" s="17" t="inlineStr">
         <is>
-          <t>卢逸</t>
+          <t>陈李石农</t>
         </is>
       </c>
       <c r="J7" s="38" t="n"/>
       <c r="K7" s="20" t="inlineStr">
         <is>
-          <t>黄婧涵</t>
+          <t>王昊天</t>
         </is>
       </c>
       <c r="L7" s="36" t="inlineStr">
         <is>
-          <t>詹悦</t>
+          <t>丁鹏元</t>
         </is>
       </c>
       <c r="M7" s="35" t="n"/>

</xml_diff>

<commit_message>
fixed should now work properly
</commit_message>
<xml_diff>
--- a/save/c5/c5 seats.xlsx
+++ b/save/c5/c5 seats.xlsx
@@ -852,7 +852,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14"/>
@@ -865,7 +865,7 @@
     <row r="1" ht="36.5" customHeight="1" s="41" thickBot="1" thickTop="1">
       <c r="A1" s="23" t="inlineStr">
         <is>
-          <t>ICC S1C5 座位表</t>
+          <t>ICC S2C5 座位表</t>
         </is>
       </c>
       <c r="B1" s="24" t="n"/>
@@ -879,7 +879,7 @@
       <c r="J1" s="24" t="n"/>
       <c r="K1" s="25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 27 Sep, 2022</t>
+          <t xml:space="preserve"> 21 Oct, 2022</t>
         </is>
       </c>
       <c r="L1" s="24" t="n"/>
@@ -930,12 +930,12 @@
       </c>
       <c r="B4" s="13" t="inlineStr">
         <is>
-          <t>林彦含</t>
+          <t>廖从云</t>
         </is>
       </c>
       <c r="C4" s="21" t="inlineStr">
         <is>
-          <t>张宸瑞</t>
+          <t>边麓元</t>
         </is>
       </c>
       <c r="D4" s="36" t="inlineStr">
@@ -945,12 +945,12 @@
       </c>
       <c r="E4" s="14" t="inlineStr">
         <is>
-          <t>迟涵予</t>
+          <t>陈元畅</t>
         </is>
       </c>
       <c r="F4" s="21" t="inlineStr">
         <is>
-          <t>蔡朋骏</t>
+          <t>詹悦</t>
         </is>
       </c>
       <c r="G4" s="36" t="inlineStr">
@@ -960,20 +960,24 @@
       </c>
       <c r="H4" s="14" t="inlineStr">
         <is>
+          <t>李星宸</t>
+        </is>
+      </c>
+      <c r="I4" s="15" t="inlineStr">
+        <is>
+          <t>龙飞宇</t>
+        </is>
+      </c>
+      <c r="J4" s="36" t="inlineStr">
+        <is>
+          <t>过道</t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="inlineStr">
+        <is>
           <t>石清泓</t>
         </is>
       </c>
-      <c r="I4" s="15" t="inlineStr">
-        <is>
-          <t>龚搏扬</t>
-        </is>
-      </c>
-      <c r="J4" s="36" t="inlineStr">
-        <is>
-          <t>过道</t>
-        </is>
-      </c>
-      <c r="K4" s="1" t="n"/>
       <c r="L4" s="32" t="n"/>
       <c r="M4" s="33" t="n"/>
     </row>
@@ -981,47 +985,43 @@
       <c r="A5" s="28" t="n"/>
       <c r="B5" s="13" t="inlineStr">
         <is>
-          <t>边麓元</t>
+          <t>王昊天</t>
         </is>
       </c>
       <c r="C5" s="14" t="inlineStr">
         <is>
-          <t>廖从云</t>
+          <t>丁鹏元</t>
         </is>
       </c>
       <c r="D5" s="37" t="n"/>
       <c r="E5" s="14" t="inlineStr">
         <is>
-          <t>王昊天</t>
+          <t>张宸瑞</t>
         </is>
       </c>
       <c r="F5" s="19" t="inlineStr">
         <is>
-          <t>丁鹏元</t>
+          <t>曾韦翔</t>
         </is>
       </c>
       <c r="G5" s="37" t="n"/>
       <c r="H5" s="14" t="inlineStr">
         <is>
-          <t>陈李石农</t>
+          <t>龚搏扬</t>
         </is>
       </c>
       <c r="I5" s="1" t="inlineStr">
         <is>
-          <t>李星宸</t>
+          <t>程启航</t>
         </is>
       </c>
       <c r="J5" s="37" t="n"/>
       <c r="K5" s="14" t="inlineStr">
         <is>
-          <t>吴周毅</t>
-        </is>
-      </c>
-      <c r="L5" s="14" t="inlineStr">
-        <is>
-          <t>卢逸</t>
-        </is>
-      </c>
+          <t>郑俊永</t>
+        </is>
+      </c>
+      <c r="L5" s="14" t="n"/>
       <c r="M5" s="34" t="inlineStr">
         <is>
           <t>墙</t>
@@ -1032,7 +1032,7 @@
       <c r="A6" s="28" t="n"/>
       <c r="B6" s="16" t="inlineStr">
         <is>
-          <t>詹悦</t>
+          <t>林彦含</t>
         </is>
       </c>
       <c r="C6" s="14" t="inlineStr">
@@ -1043,34 +1043,34 @@
       <c r="D6" s="37" t="n"/>
       <c r="E6" s="19" t="inlineStr">
         <is>
-          <t>曾韦翔</t>
+          <t>范青桐</t>
         </is>
       </c>
       <c r="F6" s="19" t="inlineStr">
         <is>
-          <t>杨熙宇</t>
+          <t>邱晨朔</t>
         </is>
       </c>
       <c r="G6" s="37" t="n"/>
       <c r="H6" s="19" t="inlineStr">
         <is>
-          <t>邱晨朔</t>
+          <t>杨熙宇</t>
         </is>
       </c>
       <c r="I6" s="19" t="inlineStr">
         <is>
-          <t>范青桐</t>
+          <t>张扬</t>
         </is>
       </c>
       <c r="J6" s="37" t="n"/>
       <c r="K6" s="19" t="inlineStr">
         <is>
-          <t>程启航</t>
+          <t>迟涵予</t>
         </is>
       </c>
       <c r="L6" s="19" t="inlineStr">
         <is>
-          <t>陈元畅</t>
+          <t>白宇轩</t>
         </is>
       </c>
       <c r="M6" s="33" t="n"/>
@@ -1079,12 +1079,12 @@
       <c r="A7" s="29" t="n"/>
       <c r="B7" s="17" t="inlineStr">
         <is>
-          <t>郑俊永</t>
+          <t>吴周毅</t>
         </is>
       </c>
       <c r="C7" s="18" t="inlineStr">
         <is>
-          <t>龙飞宇</t>
+          <t>卢逸</t>
         </is>
       </c>
       <c r="D7" s="38" t="n"/>
@@ -1112,12 +1112,12 @@
       <c r="J7" s="38" t="n"/>
       <c r="K7" s="20" t="inlineStr">
         <is>
-          <t>白宇轩</t>
+          <t>蔡朋骏</t>
         </is>
       </c>
       <c r="L7" s="36" t="inlineStr">
         <is>
-          <t>张扬</t>
+          <t>陈李石农</t>
         </is>
       </c>
       <c r="M7" s="35" t="n"/>

</xml_diff>